<commit_message>
Add stopword to list
</commit_message>
<xml_diff>
--- a/Stopwords.xlsx
+++ b/Stopwords.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="2330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="2333">
   <si>
     <t>لي</t>
   </si>
@@ -7155,6 +7155,15 @@
   </si>
   <si>
     <t>naya</t>
+  </si>
+  <si>
+    <t>na7na</t>
+  </si>
+  <si>
+    <t>houoi</t>
+  </si>
+  <si>
+    <t>hakomli</t>
   </si>
 </sst>
 </file>
@@ -7520,7 +7529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7528,10 +7537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2090"/>
+  <dimension ref="A1:A2093"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2077" workbookViewId="0">
-      <selection activeCell="A2091" sqref="A2091"/>
+    <sheetView tabSelected="1" topLeftCell="A2078" workbookViewId="0">
+      <selection activeCell="A2094" sqref="A2094"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17987,6 +17996,21 @@
     <row r="2090" spans="1:1" ht="20.25">
       <c r="A2090" s="3" t="s">
         <v>2329</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:1" ht="20.25">
+      <c r="A2091" s="3" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:1" ht="20.25">
+      <c r="A2092" s="3" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:1" ht="20.25">
+      <c r="A2093" s="3" t="s">
+        <v>2332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>